<commit_message>
Updated data to reflect claude searching ability
</commit_message>
<xml_diff>
--- a/data/venue-pricing.xlsx
+++ b/data/venue-pricing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nert/Documents/GitHub/gcal-mcp-server/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C071ED4-203C-D34E-A71C-0FA6E126DDA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFE5A2B-701C-6A47-BB37-F9D19C52B1CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Venue" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Venue!$A$1:$Z$986</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Venue!$A$1:$Z$985</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Venue</t>
   </si>
@@ -406,10 +406,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B986"/>
+  <dimension ref="A1:B985"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -579,40 +579,40 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" t="s">
-        <v>19</v>
+      <c r="A21" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="B21" s="3">
-        <v>30</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="2" t="s">
-        <v>20</v>
+      <c r="A22" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="B22" s="3">
         <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="4" t="s">
-        <v>21</v>
+      <c r="A23" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B23" s="3">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" s="3">
-        <v>100</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" s="3">
         <v>40</v>
@@ -620,19 +620,15 @@
     </row>
     <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" s="3">
-        <v>40</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="3">
-        <v>80</v>
-      </c>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="2"/>
@@ -762,7 +758,7 @@
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
     </row>
-    <row r="60" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
     </row>
@@ -4466,12 +4462,8 @@
       <c r="A985" s="2"/>
       <c r="B985" s="2"/>
     </row>
-    <row r="986" spans="1:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="A986" s="2"/>
-      <c r="B986" s="2"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:Z986" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:Z985" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>

</xml_diff>